<commit_message>
Just updated the procedures I had added
</commit_message>
<xml_diff>
--- a/Resources/User Stories.xlsx
+++ b/Resources/User Stories.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/FriendsLendsRepo/Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DBproject\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704AD5E7-1632-4815-91DD-3AAA579AFF66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stored Procedures" sheetId="1" r:id="rId1"/>
@@ -412,23 +413,23 @@
   <si>
     <t>select Headline
 from items
-where item name IN ('watering can')</t>
+where category = 'outdoors'</t>
   </si>
   <si>
     <t>select Headline
 from items
-order by item name ASC</t>
+where Headline IN ('watering can')</t>
   </si>
   <si>
     <t>select Headline
 from items
-where category = 'outdoors'</t>
+order by Headline ASC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -690,6 +691,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -957,26 +961,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.5" style="3" customWidth="1"/>
     <col min="2" max="2" width="31" style="3" customWidth="1"/>
     <col min="3" max="3" width="39.5" style="3" customWidth="1"/>
     <col min="4" max="4" width="81" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="81" style="3" customWidth="1"/>
-    <col min="6" max="6" width="51.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="51.296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -996,7 +1000,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="192" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
@@ -1016,7 +1020,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
@@ -1032,7 +1036,7 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
@@ -1048,7 +1052,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -1064,7 +1068,7 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
@@ -1078,7 +1082,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
@@ -1092,7 +1096,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
@@ -1106,7 +1110,7 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
@@ -1120,7 +1124,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
@@ -1136,7 +1140,7 @@
       </c>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
@@ -1150,7 +1154,7 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
@@ -1164,7 +1168,7 @@
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>9</v>
       </c>
@@ -1178,7 +1182,7 @@
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
@@ -1187,14 +1191,14 @@
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>9</v>
       </c>
@@ -1203,14 +1207,14 @@
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="78" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>9</v>
       </c>
@@ -1219,14 +1223,14 @@
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="176" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="171.6" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>9</v>
       </c>
@@ -1242,7 +1246,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="176" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="171.6" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="19"/>
       <c r="C18" s="19"/>
@@ -1254,7 +1258,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="17"/>
       <c r="B19" s="20"/>
       <c r="C19" s="20"/>
@@ -1264,7 +1268,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="192" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>9</v>
       </c>
@@ -1278,7 +1282,7 @@
       </c>
       <c r="F20" s="7"/>
     </row>
-    <row r="21" spans="1:6" ht="409" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>10</v>
       </c>
@@ -1292,13 +1296,13 @@
       </c>
       <c r="F21" s="7"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B23" s="4"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B25" s="4"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B27" s="4"/>
     </row>
   </sheetData>
@@ -1314,22 +1318,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="73.33203125" customWidth="1"/>
+    <col min="1" max="1" width="10.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="73.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1343,7 +1347,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" s="1" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
@@ -1355,7 +1359,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" s="1" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
@@ -1369,7 +1373,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
@@ -1389,23 +1393,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="28.1640625" customWidth="1"/>
+    <col min="2" max="2" width="28.19921875" customWidth="1"/>
     <col min="3" max="3" width="22.5" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.83203125" customWidth="1"/>
+    <col min="4" max="4" width="9.796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -1422,7 +1426,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>9</v>
       </c>
@@ -1435,7 +1439,7 @@
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
@@ -1450,7 +1454,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
@@ -1465,7 +1469,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" s="1" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -1478,7 +1482,7 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" s="1" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
@@ -1491,7 +1495,7 @@
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" s="1" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>10</v>
       </c>

</xml_diff>